<commit_message>
Working on magnetic field maps
</commit_message>
<xml_diff>
--- a/Density Depletion Project/Photoelectric Effect.xlsx
+++ b/Density Depletion Project/Photoelectric Effect.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Hughes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dehug\PycharmProjects\Mars-Research\Density Depletion Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE1299D1-63B3-4A42-A1E9-DD494615FBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECFEDC3-C2B5-431F-AB7E-75D26384C9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6BB65C6-95FA-4396-B743-5EE136AE2778}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{B6BB65C6-95FA-4396-B743-5EE136AE2778}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1443,13 +1443,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A9CEEE-B3B6-40BF-BCB2-B94C88024919}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>365</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>404.7</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>435.8</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>546.1</v>
       </c>
@@ -1661,7 +1661,6 @@
         <v>207</v>
       </c>
       <c r="N6">
-        <f>1+N5</f>
         <v>1</v>
       </c>
       <c r="O6">
@@ -1674,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>577</v>
       </c>
@@ -1705,7 +1704,6 @@
         <v>386</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N36" si="2">1+N6</f>
         <v>2</v>
       </c>
       <c r="O7">
@@ -1726,7 +1724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>3.2</v>
       </c>
@@ -1748,28 +1746,27 @@
         <v>571</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O8">
         <v>177</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8:Q25" si="3">Q7+4</f>
+        <f t="shared" ref="Q8:Q13" si="2">Q7+4</f>
         <v>8</v>
       </c>
       <c r="R8">
         <v>66</v>
       </c>
       <c r="T8">
-        <f t="shared" ref="T8:T11" si="4">4+T7</f>
+        <f t="shared" ref="T8:T11" si="3">4+T7</f>
         <v>12</v>
       </c>
       <c r="U8">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>4.2</v>
       </c>
@@ -1791,25 +1788,27 @@
         <v>688</v>
       </c>
       <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>252</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="R9">
         <v>85</v>
       </c>
       <c r="T9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="U9">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>5.2</v>
       </c>
@@ -1831,25 +1830,27 @@
         <v>774</v>
       </c>
       <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>340</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="R10">
         <v>98</v>
       </c>
       <c r="T10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="U10">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>6.2</v>
       </c>
@@ -1871,25 +1872,27 @@
         <v>843</v>
       </c>
       <c r="N11">
+        <v>15</v>
+      </c>
+      <c r="O11">
+        <v>423</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="R11">
         <v>108</v>
       </c>
       <c r="T11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="U11">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>7.2</v>
       </c>
@@ -1911,14 +1914,13 @@
         <v>925</v>
       </c>
       <c r="N12">
+        <v>19</v>
+      </c>
+      <c r="O12">
+        <v>495</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="O12">
-        <v>252</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="R12">
@@ -1932,7 +1934,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>8.1999999999999993</v>
       </c>
@@ -1954,11 +1956,13 @@
         <v>1010</v>
       </c>
       <c r="N13">
+        <v>23</v>
+      </c>
+      <c r="O13">
+        <v>554</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="R13">
@@ -1971,7 +1975,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>9.1999999999999993</v>
       </c>
@@ -1993,11 +1997,13 @@
         <v>1090</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="O14">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>10.199999999999999</v>
       </c>
@@ -2019,11 +2025,13 @@
         <v>1155</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="O15">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>11.2</v>
       </c>
@@ -2044,15 +2052,8 @@
       <c r="L16">
         <v>1227</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="O16">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>12.2</v>
       </c>
@@ -2073,12 +2074,8 @@
       <c r="L17">
         <v>1342</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>13.2</v>
       </c>
@@ -2099,12 +2096,8 @@
       <c r="L18">
         <v>1425</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>14.2</v>
       </c>
@@ -2125,12 +2118,8 @@
       <c r="L19">
         <v>1520</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>15.2</v>
       </c>
@@ -2151,15 +2140,8 @@
       <c r="L20">
         <v>1595</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="O20">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>16.2</v>
       </c>
@@ -2180,12 +2162,8 @@
       <c r="L21">
         <v>1663</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>17.2</v>
       </c>
@@ -2206,12 +2184,8 @@
       <c r="L22">
         <v>1725</v>
       </c>
-      <c r="N22">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>18.2</v>
       </c>
@@ -2232,12 +2206,8 @@
       <c r="L23">
         <v>1790</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>19.2</v>
       </c>
@@ -2258,15 +2228,8 @@
       <c r="L24">
         <v>1855</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="O24">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>20.2</v>
       </c>
@@ -2287,12 +2250,8 @@
       <c r="L25">
         <v>1905</v>
       </c>
-      <c r="N25">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>21.2</v>
       </c>
@@ -2313,12 +2272,8 @@
       <c r="L26">
         <v>1960</v>
       </c>
-      <c r="N26">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>22.2</v>
       </c>
@@ -2339,12 +2294,8 @@
       <c r="L27">
         <v>1980</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>23.2</v>
       </c>
@@ -2365,15 +2316,8 @@
       <c r="L28">
         <v>2030</v>
       </c>
-      <c r="N28">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="O28">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>24.2</v>
       </c>
@@ -2394,12 +2338,8 @@
       <c r="L29">
         <v>2070</v>
       </c>
-      <c r="N29">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>25.2</v>
       </c>
@@ -2420,12 +2360,8 @@
       <c r="L30">
         <v>2120</v>
       </c>
-      <c r="N30">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>26.2</v>
       </c>
@@ -2446,12 +2382,8 @@
       <c r="L31">
         <v>2160</v>
       </c>
-      <c r="N31">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>27.2</v>
       </c>
@@ -2472,15 +2404,8 @@
       <c r="L32">
         <v>2210</v>
       </c>
-      <c r="N32">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="O32">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>28.2</v>
       </c>
@@ -2501,12 +2426,8 @@
       <c r="L33">
         <v>2240</v>
       </c>
-      <c r="N33">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>29.2</v>
       </c>
@@ -2527,12 +2448,8 @@
       <c r="L34">
         <v>2280</v>
       </c>
-      <c r="N34">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>30.2</v>
       </c>
@@ -2553,12 +2470,8 @@
       <c r="L35">
         <v>2310</v>
       </c>
-      <c r="N35">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>31.2</v>
       </c>
@@ -2578,13 +2491,6 @@
       </c>
       <c r="L36">
         <v>2330</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="O36">
-        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>